<commit_message>
Add SourceManager to work with KeySources, rework variable sysstem, now we have only kvar and VariableType
</commit_message>
<xml_diff>
--- a/Assets/locales.xlsx
+++ b/Assets/locales.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Karen\Karen\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B977085-4C06-4B8A-8D84-99F36DD25C14}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D67026-0814-4728-88CF-24E1995C3062}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" xr2:uid="{7797A911-1672-45A9-8432-DFB14D8FC61B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" activeTab="3" xr2:uid="{7797A911-1672-45A9-8432-DFB14D8FC61B}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
     <sheet name="keys" sheetId="5" r:id="rId2"/>
     <sheet name="sample_translation_list" sheetId="4" r:id="rId3"/>
-    <sheet name="en" sheetId="2" r:id="rId4"/>
-    <sheet name="ru" sheetId="3" r:id="rId5"/>
+    <sheet name="en-US" sheetId="2" r:id="rId4"/>
+    <sheet name="ru-RU" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,10 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
-  <si>
-    <t>en</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
   <si>
     <t>hi</t>
   </si>
@@ -43,9 +40,6 @@
     <t>yes</t>
   </si>
   <si>
-    <t>ru</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -119,6 +113,15 @@
   </si>
   <si>
     <t>Форма пионера из 1980 года</t>
+  </si>
+  <si>
+    <t>You can find culture codes in https://lonewolfonline.net/list-net-culture-country-codes/</t>
+  </si>
+  <si>
+    <t>ru-RU</t>
+  </si>
+  <si>
+    <t>en-US</t>
   </si>
 </sst>
 </file>
@@ -155,7 +158,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -164,6 +167,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -484,10 +490,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{158FCD2E-233D-4BF7-8822-D4BC0046F68A}">
   <sheetPr codeName="Лист1"/>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,24 +502,36 @@
     <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B1" s="3">
         <v>2</v>
       </c>
       <c r="C1" s="3"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3">
         <v>7</v>
@@ -526,15 +544,15 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -543,7 +561,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -552,6 +570,9 @@
       <c r="K4" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D1:S1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -562,7 +583,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A4:A7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,7 +594,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1">
         <v>1</v>
@@ -581,7 +602,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -589,7 +610,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -597,7 +618,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
@@ -605,7 +626,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
@@ -613,7 +634,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1">
         <v>2</v>
@@ -621,7 +642,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1">
         <v>2</v>
@@ -653,125 +674,125 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
+        <v>8</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -783,8 +804,8 @@
   <sheetPr codeName="Лист4"/>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A4:B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -796,58 +817,58 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -873,58 +894,58 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
now game save when we quit from his
</commit_message>
<xml_diff>
--- a/Assets/locales.xlsx
+++ b/Assets/locales.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20390"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
   <workbookPr codeName="ЭтаКнига" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Karen\Karen\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D67026-0814-4728-88CF-24E1995C3062}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E41E80-C98C-4231-AB51-AD9EB09A6185}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" activeTab="3" xr2:uid="{7797A911-1672-45A9-8432-DFB14D8FC61B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" xr2:uid="{7797A911-1672-45A9-8432-DFB14D8FC61B}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
   <si>
     <t>hi</t>
   </si>
@@ -122,6 +122,18 @@
   </si>
   <si>
     <t>en-US</t>
+  </si>
+  <si>
+    <t>yes this is a pizdes</t>
+  </si>
+  <si>
+    <t>cant_ignore</t>
+  </si>
+  <si>
+    <t>You can`t ignore me!</t>
+  </si>
+  <si>
+    <t>Ты не можешь меня игнорировать!</t>
   </si>
 </sst>
 </file>
@@ -170,10 +182,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -492,8 +504,8 @@
   <sheetPr codeName="Лист1"/>
   <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,39 +522,51 @@
         <v>2</v>
       </c>
       <c r="C1" s="3"/>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="D2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -570,8 +594,9 @@
       <c r="K4" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="D1:S1"/>
+    <mergeCell ref="D2:S2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -580,10 +605,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{688735EB-3764-42C5-B958-650420E4C145}">
   <sheetPr codeName="Лист2"/>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,6 +671,14 @@
       </c>
       <c r="B7" s="1">
         <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="1">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -679,48 +712,48 @@
       <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -729,70 +762,70 @@
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -802,10 +835,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5962927B-DEDA-4BD5-86AF-ACF032952932}">
   <sheetPr codeName="Лист4"/>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,6 +904,14 @@
         <v>23</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -879,10 +920,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{582D1692-6941-4924-B0C2-658BDB0DDCC7}">
   <sheetPr codeName="Лист5"/>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -948,6 +989,14 @@
         <v>27</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add completed event when we open notepad
</commit_message>
<xml_diff>
--- a/Assets/locales.xlsx
+++ b/Assets/locales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Karen\Karen\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E41E80-C98C-4231-AB51-AD9EB09A6185}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFFD07C5-9698-4D44-B956-9BDA283FDE1B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" xr2:uid="{7797A911-1672-45A9-8432-DFB14D8FC61B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" activeTab="4" xr2:uid="{7797A911-1672-45A9-8432-DFB14D8FC61B}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
   <si>
     <t>hi</t>
   </si>
@@ -134,6 +134,24 @@
   </si>
   <si>
     <t>Ты не можешь меня игнорировать!</t>
+  </si>
+  <si>
+    <t>notepad_1</t>
+  </si>
+  <si>
+    <t>notepad_2</t>
+  </si>
+  <si>
+    <t>Эй, ты открыл блокнот?</t>
+  </si>
+  <si>
+    <t>А зачем?</t>
+  </si>
+  <si>
+    <t>Do you open notepad?</t>
+  </si>
+  <si>
+    <t>But why?</t>
   </si>
 </sst>
 </file>
@@ -170,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -183,6 +201,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -504,7 +525,7 @@
   <sheetPr codeName="Лист1"/>
   <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -522,51 +543,51 @@
         <v>2</v>
       </c>
       <c r="C1" s="3"/>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="3">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -605,10 +626,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{688735EB-3764-42C5-B958-650420E4C145}">
   <sheetPr codeName="Лист2"/>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,6 +700,22 @@
       </c>
       <c r="B8" s="1">
         <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="1">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -835,10 +872,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5962927B-DEDA-4BD5-86AF-ACF032952932}">
   <sheetPr codeName="Лист4"/>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -912,6 +949,22 @@
         <v>33</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -920,10 +973,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{582D1692-6941-4924-B0C2-658BDB0DDCC7}">
   <sheetPr codeName="Лист5"/>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -997,6 +1050,22 @@
         <v>34</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
delete not used keys
</commit_message>
<xml_diff>
--- a/Assets/locales.xlsx
+++ b/Assets/locales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Karen\Karen\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFFD07C5-9698-4D44-B956-9BDA283FDE1B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C262D62-13E8-4A20-82F1-6316AE77EDA2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" activeTab="4" xr2:uid="{7797A911-1672-45A9-8432-DFB14D8FC61B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" activeTab="1" xr2:uid="{7797A911-1672-45A9-8432-DFB14D8FC61B}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -29,29 +29,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>hi</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Да</t>
-  </si>
-  <si>
-    <t>Нет</t>
-  </si>
-  <si>
     <t>key</t>
   </si>
   <si>
@@ -77,42 +59,6 @@
   </si>
   <si>
     <t>Привет!</t>
-  </si>
-  <si>
-    <t>karen</t>
-  </si>
-  <si>
-    <t>karen_hair</t>
-  </si>
-  <si>
-    <t>karen_eyes</t>
-  </si>
-  <si>
-    <t>karen_clothes</t>
-  </si>
-  <si>
-    <t>Karen</t>
-  </si>
-  <si>
-    <t>Light-blue hair</t>
-  </si>
-  <si>
-    <t>Its two</t>
-  </si>
-  <si>
-    <t>Pioneer form from 1980 year</t>
-  </si>
-  <si>
-    <t>Карен</t>
-  </si>
-  <si>
-    <t>Голубые волосы</t>
-  </si>
-  <si>
-    <t>Их два</t>
-  </si>
-  <si>
-    <t>Форма пионера из 1980 года</t>
   </si>
   <si>
     <t>You can find culture codes in https://lonewolfonline.net/list-net-culture-country-codes/</t>
@@ -526,7 +472,7 @@
   <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,14 +483,14 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B1" s="3">
         <v>2</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="6" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
@@ -564,14 +510,14 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="6" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
@@ -591,13 +537,13 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -626,10 +572,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{688735EB-3764-42C5-B958-650420E4C145}">
   <sheetPr codeName="Лист2"/>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,78 +594,30 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="1">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState ref="A1:B6">
+  <sortState ref="A1:B1">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -744,10 +642,10 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -794,10 +692,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -872,10 +770,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5962927B-DEDA-4BD5-86AF-ACF032952932}">
   <sheetPr codeName="Лист4"/>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B2" sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -887,82 +785,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>14</v>
+      <c r="A3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B4" s="5" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -973,10 +823,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{582D1692-6941-4924-B0C2-658BDB0DDCC7}">
   <sheetPr codeName="Лист5"/>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,82 +838,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add resume script, and SEP for him; remove async.miku and not used locales; other engine changes
</commit_message>
<xml_diff>
--- a/Assets/locales.xlsx
+++ b/Assets/locales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Karen\Karen\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C262D62-13E8-4A20-82F1-6316AE77EDA2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F749027-E9E4-42CD-8143-EAC7A6D68321}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" activeTab="1" xr2:uid="{7797A911-1672-45A9-8432-DFB14D8FC61B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" activeTab="4" xr2:uid="{7797A911-1672-45A9-8432-DFB14D8FC61B}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="ru-RU" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
   <si>
     <t>hi</t>
   </si>
@@ -98,6 +99,60 @@
   </si>
   <si>
     <t>But why?</t>
+  </si>
+  <si>
+    <t>resume_1_1</t>
+  </si>
+  <si>
+    <t>resume_1_2</t>
+  </si>
+  <si>
+    <t>resume_1_3</t>
+  </si>
+  <si>
+    <t>resume_2_1</t>
+  </si>
+  <si>
+    <t>resume_2_2</t>
+  </si>
+  <si>
+    <t>О, ты вернулся!</t>
+  </si>
+  <si>
+    <t>Как дела?</t>
+  </si>
+  <si>
+    <t>Т-ты скучал по мне?</t>
+  </si>
+  <si>
+    <t>С возращением, Семпай❤!</t>
+  </si>
+  <si>
+    <t>И?</t>
+  </si>
+  <si>
+    <t>Тебе это понравилось?</t>
+  </si>
+  <si>
+    <t>resume_2_3</t>
+  </si>
+  <si>
+    <t>Oh, you're back!</t>
+  </si>
+  <si>
+    <t>How is it going?</t>
+  </si>
+  <si>
+    <t>D-did you missed me?</t>
+  </si>
+  <si>
+    <t>Welcome back, Sempai❤!</t>
+  </si>
+  <si>
+    <t>And?</t>
+  </si>
+  <si>
+    <t>Did you like it?</t>
   </si>
 </sst>
 </file>
@@ -134,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -147,6 +202,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -472,7 +530,7 @@
   <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,51 +547,51 @@
         <v>2</v>
       </c>
       <c r="C1" s="3"/>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="3">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -572,10 +630,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{688735EB-3764-42C5-B958-650420E4C145}">
   <sheetPr codeName="Лист2"/>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,6 +672,54 @@
       </c>
       <c r="B4" s="1">
         <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="1">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -770,10 +876,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5962927B-DEDA-4BD5-86AF-ACF032952932}">
   <sheetPr codeName="Лист4"/>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="A1:B2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,6 +921,54 @@
         <v>22</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -823,10 +977,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{582D1692-6941-4924-B0C2-658BDB0DDCC7}">
   <sheetPr codeName="Лист5"/>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="A1:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,6 +1022,54 @@
         <v>20</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add event when cmd open
</commit_message>
<xml_diff>
--- a/Assets/locales.xlsx
+++ b/Assets/locales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Karen\Karen\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E81AC3-97E5-4D0C-BD4E-41B857F86D3D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F338A90-AF95-4005-A6FA-C71686154573}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" xr2:uid="{7797A911-1672-45A9-8432-DFB14D8FC61B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" activeTab="4" xr2:uid="{7797A911-1672-45A9-8432-DFB14D8FC61B}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="100">
   <si>
     <t>hi</t>
   </si>
@@ -293,6 +293,42 @@
   </si>
   <si>
     <t>Do something else for now, I`ll be right back…</t>
+  </si>
+  <si>
+    <t>cmd_1</t>
+  </si>
+  <si>
+    <t>cmd_2</t>
+  </si>
+  <si>
+    <t>cmd_3</t>
+  </si>
+  <si>
+    <t>cmd_4</t>
+  </si>
+  <si>
+    <t>Ты открыл консоль?</t>
+  </si>
+  <si>
+    <t>Попробуй нажать в ней Alt+Enter</t>
+  </si>
+  <si>
+    <t>А потом ещё раз.</t>
+  </si>
+  <si>
+    <t>Если, конечно, не боишься.</t>
+  </si>
+  <si>
+    <t>Do you open a console?</t>
+  </si>
+  <si>
+    <t>Try to press Alt+Enter in console window.</t>
+  </si>
+  <si>
+    <t>And then again.</t>
+  </si>
+  <si>
+    <t>Unless yor`re afraid, of course.</t>
   </si>
 </sst>
 </file>
@@ -672,7 +708,7 @@
   <sheetPr codeName="Лист1"/>
   <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -714,7 +750,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="3">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="8" t="s">
@@ -773,10 +809,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{688735EB-3764-42C5-B958-650420E4C145}">
   <sheetPr codeName="Лист2"/>
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B31" sqref="A28:B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,6 +1035,38 @@
       </c>
       <c r="B27" s="7">
         <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B29" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B31" s="7">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1155,10 +1223,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5962927B-DEDA-4BD5-86AF-ACF032952932}">
   <sheetPr codeName="Лист4"/>
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1384,6 +1452,38 @@
         <v>87</v>
       </c>
     </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1392,10 +1492,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{582D1692-6941-4924-B0C2-658BDB0DDCC7}">
   <sheetPr codeName="Лист5"/>
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1621,6 +1721,38 @@
         <v>72</v>
       </c>
     </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add event when regedit open
</commit_message>
<xml_diff>
--- a/Assets/locales.xlsx
+++ b/Assets/locales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Karen\Karen\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F338A90-AF95-4005-A6FA-C71686154573}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F2E9CA-0A7C-4B6B-BFEB-1DAD6D92175D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" activeTab="4" xr2:uid="{7797A911-1672-45A9-8432-DFB14D8FC61B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" activeTab="3" xr2:uid="{7797A911-1672-45A9-8432-DFB14D8FC61B}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="106">
   <si>
     <t>hi</t>
   </si>
@@ -329,6 +329,24 @@
   </si>
   <si>
     <t>Unless yor`re afraid, of course.</t>
+  </si>
+  <si>
+    <t>reg_1</t>
+  </si>
+  <si>
+    <t>reg_2</t>
+  </si>
+  <si>
+    <t>Если честно, то я уже сделала пару записей в реестре.</t>
+  </si>
+  <si>
+    <t>Поищи их, если хочешь.</t>
+  </si>
+  <si>
+    <t>To be honest, I have already made a couple entries in the registry.</t>
+  </si>
+  <si>
+    <t>If you want, try to find and look for them.</t>
   </si>
 </sst>
 </file>
@@ -809,10 +827,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{688735EB-3764-42C5-B958-650420E4C145}">
   <sheetPr codeName="Лист2"/>
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B31" sqref="A28:B31"/>
+      <selection activeCell="B33" sqref="A32:B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1066,6 +1084,22 @@
         <v>91</v>
       </c>
       <c r="B31" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" s="1">
         <v>4</v>
       </c>
     </row>
@@ -1223,16 +1257,16 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5962927B-DEDA-4BD5-86AF-ACF032952932}">
   <sheetPr codeName="Лист4"/>
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="51.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="64" style="1" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -1482,6 +1516,22 @@
       </c>
       <c r="B31" s="7" t="s">
         <v>99</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1492,10 +1542,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{582D1692-6941-4924-B0C2-658BDB0DDCC7}">
   <sheetPr codeName="Лист5"/>
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1753,6 +1803,22 @@
         <v>95</v>
       </c>
     </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add source code random evvent
</commit_message>
<xml_diff>
--- a/Assets/locales.xlsx
+++ b/Assets/locales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Karen\Karen\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F2E9CA-0A7C-4B6B-BFEB-1DAD6D92175D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB20489D-B205-4A3A-BF23-0D86A341F9C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" activeTab="3" xr2:uid="{7797A911-1672-45A9-8432-DFB14D8FC61B}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="115">
   <si>
     <t>hi</t>
   </si>
@@ -347,6 +347,33 @@
   </si>
   <si>
     <t>If you want, try to find and look for them.</t>
+  </si>
+  <si>
+    <t>source_code_1</t>
+  </si>
+  <si>
+    <t>source_code_2</t>
+  </si>
+  <si>
+    <t>source_code_3</t>
+  </si>
+  <si>
+    <t>Если да, то ты можешь найти мой исходный код по адресу https://github.com/lesh6295-png/Karen</t>
+  </si>
+  <si>
+    <t>Быть может, ты найдёшь там что-нибудь интерестное.</t>
+  </si>
+  <si>
+    <t>А ты разбираешься в электронике?</t>
+  </si>
+  <si>
+    <t>If yes, you can find my source code in https://github.com/lesh6295-png/Karen</t>
+  </si>
+  <si>
+    <t>Are you into coding?</t>
+  </si>
+  <si>
+    <t>Maybe, you can find something interesting</t>
   </si>
 </sst>
 </file>
@@ -383,7 +410,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -396,6 +423,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -744,51 +774,51 @@
         <v>2</v>
       </c>
       <c r="C1" s="3"/>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="3">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -827,10 +857,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{688735EB-3764-42C5-B958-650420E4C145}">
   <sheetPr codeName="Лист2"/>
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B33" sqref="A32:B33"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1101,6 +1131,30 @@
       </c>
       <c r="B33" s="1">
         <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B34" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B35" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B36" s="1">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1257,16 +1311,16 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5962927B-DEDA-4BD5-86AF-ACF032952932}">
   <sheetPr codeName="Лист4"/>
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="64" style="1" customWidth="1"/>
+    <col min="2" max="2" width="98" style="1" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -1532,6 +1586,30 @@
       </c>
       <c r="B33" s="7" t="s">
         <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1542,16 +1620,16 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{582D1692-6941-4924-B0C2-658BDB0DDCC7}">
   <sheetPr codeName="Лист5"/>
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="B36" sqref="A34:B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="59" style="1" customWidth="1"/>
+    <col min="2" max="2" width="101.85546875" style="1" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -1819,6 +1897,30 @@
         <v>103</v>
       </c>
     </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>